<commit_message>
this is new modify code for excel update in 14/06/2024
</commit_message>
<xml_diff>
--- a/Externaldata/BimsDataAuto1.xlsx
+++ b/Externaldata/BimsDataAuto1.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulu satapathy\Desktop\Work\Oasys\Externaldata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirak\Desktop\Radhakrushna_OASYS\OasysApp\Oasys\Externaldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAA5184-D122-4A10-A1A1-C06DC36C003A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C2A97-4424-465B-92BA-0E392463C319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B33D0FC7-30BD-46C7-B0C2-78BA204C6A8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B33D0FC7-30BD-46C7-B0C2-78BA204C6A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>BoatOwnerId</t>
   </si>
@@ -147,13 +147,29 @@
     <t>OrangeContact number is already in use. apple</t>
   </si>
   <si>
-    <t>Contact number is already in use.</t>
+    <t>PRASANN</t>
+  </si>
+  <si>
+    <t>TARA</t>
+  </si>
+  <si>
+    <t>PRASA</t>
+  </si>
+  <si>
+    <t>TAR</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>OrangeOops... apple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -552,32 +568,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE56C20E-B7EB-4450-856F-8708189ECAE0}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="31.36328125" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" customWidth="1"/>
-    <col min="12" max="12" width="38.08984375" customWidth="1"/>
-    <col min="30" max="30" width="21.81640625" customWidth="1"/>
-    <col min="31" max="31" width="18.90625" customWidth="1"/>
-    <col min="32" max="32" width="48.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.77734375"/>
+    <col min="2" max="2" customWidth="true" width="23.44140625"/>
+    <col min="3" max="3" customWidth="true" width="20.21875"/>
+    <col min="4" max="4" customWidth="true" width="15.88671875"/>
+    <col min="5" max="5" customWidth="true" width="18.21875"/>
+    <col min="6" max="6" customWidth="true" width="16.6640625"/>
+    <col min="7" max="7" customWidth="true" width="14.33203125"/>
+    <col min="8" max="8" customWidth="true" width="16.0"/>
+    <col min="9" max="9" customWidth="true" width="31.33203125"/>
+    <col min="10" max="10" customWidth="true" width="20.21875"/>
+    <col min="11" max="11" customWidth="true" width="19.109375"/>
+    <col min="12" max="12" customWidth="true" width="38.109375"/>
+    <col min="30" max="30" customWidth="true" width="21.77734375"/>
+    <col min="31" max="31" customWidth="true" width="18.88671875"/>
+    <col min="32" max="32" customWidth="true" width="48.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +691,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>6403</v>
       </c>
@@ -698,7 +714,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="2">
-        <v>6372602822</v>
+        <v>6372602823</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>32</v>
@@ -726,10 +742,10 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>6405</v>
       </c>
@@ -783,7 +799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>6405</v>
       </c>
@@ -806,7 +822,7 @@
         <v>36</v>
       </c>
       <c r="H4" s="2">
-        <v>8328961274</v>
+        <v>8328961074</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>37</v>
@@ -837,6 +853,168 @@
         <v>39</v>
       </c>
     </row>
+    <row r="5" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>6405</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4">
+        <v>112</v>
+      </c>
+      <c r="F5" s="5">
+        <v>234</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8324961274</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>6405</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4">
+        <v>112</v>
+      </c>
+      <c r="F6" s="5">
+        <v>234</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8324961274</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6405</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4">
+        <v>112</v>
+      </c>
+      <c r="F7" s="5">
+        <v>234</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8324960276</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>